<commit_message>
organized the analysis sheet
</commit_message>
<xml_diff>
--- a/Amazon-bestbooksellers-with-categories-2024-02-02.xlsx
+++ b/Amazon-bestbooksellers-with-categories-2024-02-02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2f83c3b872d77321/Desktop/github-projects-data-analysis-ms-excel/Amazon-bestbooksellers-with-categories-data-analysis-ms-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1674" documentId="13_ncr:40009_{860ED095-479F-4D58-ADB2-4B8FA8E775F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A113C6A2-B3BF-4EFF-8C7F-7307722416CD}"/>
+  <xr:revisionPtr revIDLastSave="1796" documentId="13_ncr:40009_{860ED095-479F-4D58-ADB2-4B8FA8E775F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A53500F-199A-48CC-98CF-DDBCABFAB28D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="534" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bestsellers with categories" sheetId="1" r:id="rId1"/>
@@ -19,19 +19,19 @@
     <sheet name="Data information" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'bestsellers with categories'!$E$2:$E$551</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'bestsellers with categories'!$E$2:$E$551</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'bestsellers with categories'!$D$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'bestsellers with categories'!$D$2:$D$551</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'bestsellers with categories'!$C$2:$C$551</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'bestsellers with categories'!$E$2:$E$551</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'bestsellers with categories'!$I$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'bestsellers with categories'!$I$2:$I$551</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'bestsellers with categories'!$E$2:$E$551</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'bestsellers with categories'!$D$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'bestsellers with categories'!$D$2:$D$551</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'bestsellers with categories'!$E$2:$E$551</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'bestsellers with categories'!$C$2:$C$551</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'bestsellers with categories'!$I$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'bestsellers with categories'!$I$2:$I$551</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'bestsellers with categories'!$E$2:$E$551</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'bestsellers with categories'!$D$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'bestsellers with categories'!$D$2:$D$551</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1993,16 +1993,10 @@
     <t>This infers that there is equal number of books are sold in each year</t>
   </si>
   <si>
-    <t>What is the trend of user rating?</t>
-  </si>
-  <si>
     <t>Max of Reviews</t>
   </si>
   <si>
     <t>This infers that Fiction genre had the highest total number of reviews</t>
-  </si>
-  <si>
-    <t>About 180 books have a rating of 4.8 or 4.9.</t>
   </si>
   <si>
     <t>Popularity Level</t>
@@ -2118,9 +2112,6 @@
     <t>Price Histogram</t>
   </si>
   <si>
-    <t>this infers that there are around 187 books that are sold with &lt; 9.2 dollars</t>
-  </si>
-  <si>
     <t>this infers that there are more non fiction books than fiction</t>
   </si>
   <si>
@@ -2128,6 +2119,15 @@
   </si>
   <si>
     <t xml:space="preserve">from this histogram we can infer that around 55% of books have the price range from 4.6 to 13.8 dollars </t>
+  </si>
+  <si>
+    <t>What is the distribution of user rating?</t>
+  </si>
+  <si>
+    <t>About 127 books have the rating between 4.755 , 4.852</t>
+  </si>
+  <si>
+    <t>This infers that there are around 187 books that are sold with &lt; 9.2 dollars</t>
   </si>
 </sst>
 </file>
@@ -3325,6 +3325,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>User rating</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3387,6 +3442,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Price</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4824,6 +4934,36 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>User</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> rating with the year </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4913,6 +5053,36 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sum</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of price</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5524,11 +5694,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -5538,13 +5708,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Average</a:t>
+              <a:t>Average price of genre books </a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> price of genre books </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5561,11 +5726,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -5582,17 +5747,41 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
+          <a:pattFill prst="ltDnDiag">
+            <a:fgClr>
+              <a:schemeClr val="accent1"/>
+            </a:fgClr>
+            <a:bgClr>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:bgClr>
+          </a:pattFill>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
-          <a:sp3d/>
+          <a:sp3d>
+            <a:contourClr>
+              <a:schemeClr val="accent1"/>
+            </a:contourClr>
+          </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -5638,15 +5827,17 @@
       </c:pivotFmt>
     </c:pivotFmts>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
+      <c:rotX val="10"/>
+      <c:rotY val="0"/>
       <c:depthPercent val="100"/>
-      <c:rAngAx val="1"/>
+      <c:rAngAx val="0"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -5697,14 +5888,28 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d>
+              <a:contourClr>
+                <a:schemeClr val="accent1"/>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -5749,14 +5954,13 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                    <a:ln w="9525">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -5807,7 +6011,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="160"/>
+        <c:gapDepth val="0"/>
         <c:shape val="box"/>
         <c:axId val="1821111119"/>
         <c:axId val="1596955887"/>
@@ -5820,6 +6025,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Genre</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5865,20 +6125,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average of price</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -11411,7 +11712,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Book with teh highest price </a:t>
+              <a:t>Book with the highest price </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -11504,6 +11805,20 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -11535,6 +11850,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-64DA-4A87-A0CB-1A2E37C77837}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -11889,37 +12225,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -11967,7 +12272,6 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -11985,18 +12289,45 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Distribution of number of reviews received</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Distribution of number of reviews received</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="clusteredColumn" uniqueId="{BCE432E1-4ABD-45B6-BCFE-F97514A08568}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Reviews</cx:v>
             </cx:txData>
           </cx:tx>
@@ -12008,10 +12339,66 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="0"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>reviews </cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>reviews </a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Count of reviews </cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Count of reviews </a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines>
           <cx:spPr>
             <a:ln w="9525" cmpd="dbl">
@@ -12033,7 +12420,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -12150,7 +12537,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -12188,7 +12575,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{8308D36D-A129-418F-BB25-874F1CAD4DB0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>length of the name</cx:v>
             </cx:txData>
           </cx:tx>
@@ -12273,7 +12660,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -12362,7 +12749,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -18185,7 +18572,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="287">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -18196,7 +18583,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -18208,6 +18595,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr/>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -18215,7 +18603,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -18231,7 +18619,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -18275,32 +18663,72 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -18312,33 +18740,29 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -18360,15 +18784,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -18378,7 +18800,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -18387,14 +18809,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -18403,10 +18824,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -18422,14 +18843,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -18441,13 +18862,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:sp3d/>
     </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
@@ -18455,17 +18876,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -18474,17 +18894,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -18493,14 +18912,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -18512,17 +18931,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -18543,7 +18961,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -18551,7 +18969,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -18571,10 +18989,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -18591,11 +19009,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -18604,14 +19022,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -18632,20 +19049,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -18666,14 +19082,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -20718,15 +21128,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>388470</xdr:colOff>
+      <xdr:colOff>207848</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>99608</xdr:rowOff>
+      <xdr:rowOff>37519</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>867335</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>146756</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>99608</xdr:rowOff>
+      <xdr:rowOff>37519</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -20762,8 +21172,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="388470" y="1440728"/>
-              <a:ext cx="3328745" cy="2743200"/>
+              <a:off x="207848" y="1375252"/>
+              <a:ext cx="3839219" cy="2709334"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -20868,15 +21278,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>772413</xdr:colOff>
-      <xdr:row>654</xdr:row>
-      <xdr:rowOff>13648</xdr:rowOff>
+      <xdr:colOff>598310</xdr:colOff>
+      <xdr:row>655</xdr:row>
+      <xdr:rowOff>2358</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1191328</xdr:colOff>
+      <xdr:colOff>959904</xdr:colOff>
       <xdr:row>666</xdr:row>
-      <xdr:rowOff>64006</xdr:rowOff>
+      <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20903,16 +21313,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>24448</xdr:colOff>
-      <xdr:row>707</xdr:row>
-      <xdr:rowOff>21901</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>154270</xdr:colOff>
+      <xdr:row>706</xdr:row>
+      <xdr:rowOff>168656</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>546506</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4640</xdr:colOff>
       <xdr:row>721</xdr:row>
-      <xdr:rowOff>169112</xdr:rowOff>
+      <xdr:rowOff>135245</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21206,15 +21616,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>821185</xdr:colOff>
-      <xdr:row>835</xdr:row>
-      <xdr:rowOff>181514</xdr:rowOff>
+      <xdr:colOff>352697</xdr:colOff>
+      <xdr:row>836</xdr:row>
+      <xdr:rowOff>57337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>967905</xdr:colOff>
-      <xdr:row>850</xdr:row>
-      <xdr:rowOff>140419</xdr:rowOff>
+      <xdr:colOff>499417</xdr:colOff>
+      <xdr:row>851</xdr:row>
+      <xdr:rowOff>33175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21319,16 +21729,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>908243</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>168820</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>110066</xdr:rowOff>
+      <xdr:rowOff>132643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>346364</xdr:colOff>
+      <xdr:colOff>656808</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>66963</xdr:rowOff>
+      <xdr:rowOff>89540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21355,16 +21765,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>169333</xdr:colOff>
-      <xdr:row>723</xdr:row>
-      <xdr:rowOff>171643</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>519288</xdr:colOff>
+      <xdr:row>724</xdr:row>
+      <xdr:rowOff>188576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>946727</xdr:colOff>
-      <xdr:row>737</xdr:row>
-      <xdr:rowOff>76970</xdr:rowOff>
+      <xdr:colOff>275038</xdr:colOff>
+      <xdr:row>738</xdr:row>
+      <xdr:rowOff>93904</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21436,8 +21846,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5249334" y="62788800"/>
-              <a:ext cx="4370702" cy="2688415"/>
+              <a:off x="5248487" y="63463593"/>
+              <a:ext cx="4366469" cy="2722282"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -27137,603 +27547,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{72F60BBE-DA90-4D37-B621-310679FC9C8B}" name="PivotTable16" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
-  <location ref="A763:B766" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Max of Reviews" fld="3" subtotal="max" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="10" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D52EFF79-3D17-4518-8D79-A4928BDC2D1F}" name="PivotTable9" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A594:B653" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item h="1" x="13"/>
-        <item h="1" x="10"/>
-        <item h="1" x="9"/>
-        <item h="1" x="5"/>
-        <item h="1" x="11"/>
-        <item h="1" x="12"/>
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
-        <item h="1" x="3"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="12">
-        <item x="7"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="8"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="6"/>
-    <field x="5"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="59">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1">
-            <x v="11"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="4">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="11"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C2258B0-8207-4FF9-800C-EBDA430C8AB4}" name="PivotTable15" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A726:B738" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="12">
-        <item x="7"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="8"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="5"/>
-  </rowFields>
-  <rowItems count="12">
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Name" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="12">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5F8312A1-0737-4D0C-B64A-F51A9D3FCBF1}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5F8312A1-0737-4D0C-B64A-F51A9D3FCBF1}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A27:B33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" measureFilter="1" sortType="descending">
@@ -28136,12 +27950,24 @@
   <dataFields count="1">
     <dataField name="Max of Price" fld="4" subtotal="max" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="56"/>
           </reference>
         </references>
       </pivotArea>
@@ -28168,8 +27994,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C70DBB2D-1B0A-4E15-91E7-5E865F4707EA}" name="PivotTable14" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C70DBB2D-1B0A-4E15-91E7-5E865F4707EA}" name="PivotTable14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A709:B712" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -28229,8 +28055,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{732C41A9-2EEB-43E4-8B0A-3ADBC3A08B9A}" name="PivotTable13" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{732C41A9-2EEB-43E4-8B0A-3ADBC3A08B9A}" name="PivotTable13" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A690:B705" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -28579,8 +28405,366 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3CA635E2-9B80-4E83-B2CB-0A89149DE567}" name="PivotTable10" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{72F60BBE-DA90-4D37-B621-310679FC9C8B}" name="PivotTable16" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="18">
+  <location ref="A763:B766" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Max of Reviews" fld="3" subtotal="max" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="10" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D52EFF79-3D17-4518-8D79-A4928BDC2D1F}" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A594:B653" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item h="1" x="13"/>
+        <item h="1" x="10"/>
+        <item h="1" x="9"/>
+        <item h="1" x="5"/>
+        <item h="1" x="11"/>
+        <item h="1" x="12"/>
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="3"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item x="7"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="6"/>
+    <field x="5"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="59">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1">
+            <x v="11"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3CA635E2-9B80-4E83-B2CB-0A89149DE567}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A656:B659" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -28664,8 +28848,246 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C2258B0-8207-4FF9-800C-EBDA430C8AB4}" name="PivotTable15" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A726:B738" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="12">
+        <item x="7"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Name" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="12">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43515F51-2C56-4B60-989D-970231CCADD5}" name="PivotTable23" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43515F51-2C56-4B60-989D-970231CCADD5}" name="PivotTable23" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A838:B849" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" measureFilter="1" sortType="descending">
@@ -29709,8 +30131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K551"/>
   <sheetViews>
-    <sheetView topLeftCell="A528" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C551"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29721,7 +30143,7 @@
     <col min="4" max="4" width="15.109375" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="23.5546875" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="33"/>
+    <col min="9" max="9" width="14.88671875" style="33" customWidth="1"/>
     <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29750,8 +30172,8 @@
       <c r="H1" t="s">
         <v>632</v>
       </c>
-      <c r="I1" s="33" t="s">
-        <v>661</v>
+      <c r="I1" s="7" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -46819,8 +47241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A253F81-9E7D-4DA8-AE55-0C5762407D7F}">
   <dimension ref="A1:H885"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A861" zoomScale="135" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="F885" sqref="F885"/>
+    <sheetView zoomScale="135" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="G885" sqref="G885"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52139,7 +52561,7 @@
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A668" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="670" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -52609,7 +53031,7 @@
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A716" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="725" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -52728,12 +53150,12 @@
     </row>
     <row r="742" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A742" s="19" t="s">
-        <v>647</v>
+        <v>682</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A759" s="51" t="s">
-        <v>650</v>
+        <v>683</v>
       </c>
     </row>
     <row r="761" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -52746,7 +53168,7 @@
         <v>619</v>
       </c>
       <c r="B763" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.3">
@@ -52775,86 +53197,86 @@
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A779" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="781" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A781" s="21" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A782" s="3" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A783" s="35" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B783" s="35" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A784" s="35" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B784" s="35" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A785" s="35" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B785" s="35" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A786" s="35" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B786" s="35" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A787" s="35" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B787" s="35" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="790" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A790" s="21" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="809" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A809" s="21" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="810" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A810" s="42" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="812" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A812" s="40"/>
       <c r="B812" s="41" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C812" s="41" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="813" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A813" s="41" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B813" s="41">
         <v>1</v>
@@ -52863,7 +53285,7 @@
     </row>
     <row r="814" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A814" s="41" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B814" s="41">
         <v>1.4527795782405852E-3</v>
@@ -52874,41 +53296,41 @@
     </row>
     <row r="816" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A816" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="825" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A825" s="43" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="827" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A827" s="42" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B827" s="42"/>
     </row>
     <row r="828" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A828" s="42" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B828" s="42"/>
     </row>
     <row r="829" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A829" s="44" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B829" s="42"/>
     </row>
     <row r="830" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A830" s="42" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B830" s="42"/>
     </row>
     <row r="831" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A831" s="42" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B831" s="42"/>
     </row>
@@ -52918,7 +53340,7 @@
     </row>
     <row r="833" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A833" s="45" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B833" s="46">
         <f>MAX('extra sheet for other analysis'!I3:I352)</f>
@@ -52927,7 +53349,7 @@
     </row>
     <row r="834" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A834" s="47" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B834" s="46" t="str">
         <f>INDEX('extra sheet for other analysis'!H3:H352,MATCH(MAX('extra sheet for other analysis'!I3:I352),'extra sheet for other analysis'!I3:I352,0))</f>
@@ -52936,7 +53358,7 @@
     </row>
     <row r="836" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A836" s="21" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.3">
@@ -52944,7 +53366,7 @@
         <v>619</v>
       </c>
       <c r="B838" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.3">
@@ -53037,15 +53459,15 @@
     </row>
     <row r="867" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A867" s="21" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="885" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A885" t="s">
+        <v>684</v>
+      </c>
+      <c r="G885" t="s">
         <v>681</v>
-      </c>
-      <c r="G885" t="s">
-        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -53070,10 +53492,10 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -53081,7 +53503,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>0</v>
@@ -53090,7 +53512,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -53325,7 +53747,7 @@
         <v>12</v>
       </c>
       <c r="N14" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -61564,7 +61986,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A3" sqref="A3:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>